<commit_message>
Changes 14 Oct 2025 Time=17.00PM
</commit_message>
<xml_diff>
--- a/public/achivements_excel/patents_data.xlsx
+++ b/public/achivements_excel/patents_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\s417\dept_website\public\achivements_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{451DBB44-14E5-4BC3-9BBF-910FC1D076DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3666CEC-23E0-4429-92FF-B472D73C03D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5C30D9FD-C1FB-46D1-8F77-CDE7C1242831}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -72,15 +72,6 @@
   </si>
   <si>
     <t>Dr. Abhishek Subramanian</t>
-  </si>
-  <si>
-    <t>International</t>
-  </si>
-  <si>
-    <t>Patent submitted</t>
-  </si>
-  <si>
-    <t>US20180371643A1</t>
   </si>
 </sst>
 </file>
@@ -455,7 +446,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +454,7 @@
     <col min="1" max="1" width="50.85546875" customWidth="1"/>
     <col min="2" max="2" width="40.140625" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,13 +574,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>454732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>